<commit_message>
merubah banyak sebelum bimbingan pertama
</commit_message>
<xml_diff>
--- a/jadwal-kerja.xlsx
+++ b/jadwal-kerja.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="jadwal-kerja" sheetId="1" r:id="rId1"/>
+    <sheet name="komputer-tersedia" sheetId="2" r:id="rId2"/>
+    <sheet name="design-tabel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="107">
   <si>
     <t>JADWAL KERJA PT TIRTAKENCANA TATAWARNA DIVISI MARKETING</t>
   </si>
@@ -169,6 +170,183 @@
   </si>
   <si>
     <t>Supervisor Divisi 2</t>
+  </si>
+  <si>
+    <t>Nama Atribute</t>
+  </si>
+  <si>
+    <t>Tipe Data</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>foto</t>
+  </si>
+  <si>
+    <t>login_session_key</t>
+  </si>
+  <si>
+    <t>auth</t>
+  </si>
+  <si>
+    <t>email_status</t>
+  </si>
+  <si>
+    <t>verify</t>
+  </si>
+  <si>
+    <t>password_expired_date</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>password_reset_key</t>
+  </si>
+  <si>
+    <t>user_role_id</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>fk user role</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>id_role</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>role permissions</t>
+  </si>
+  <si>
+    <t>id_role_permissions</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>page_name</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>action_name</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>act</t>
+  </si>
+  <si>
+    <t>gejala</t>
+  </si>
+  <si>
+    <t>aturan</t>
+  </si>
+  <si>
+    <t>diagnosa</t>
+  </si>
+  <si>
+    <t>kerusakan</t>
+  </si>
+  <si>
+    <t>solusi</t>
+  </si>
+  <si>
+    <t>id_gejala</t>
+  </si>
+  <si>
+    <t>nama_gejala</t>
+  </si>
+  <si>
+    <t>aturan_id</t>
+  </si>
+  <si>
+    <t>id_aturan</t>
+  </si>
+  <si>
+    <t>fk rolepermission role</t>
+  </si>
+  <si>
+    <t>fk gejala aturan</t>
+  </si>
+  <si>
+    <t>gejala_id</t>
+  </si>
+  <si>
+    <t>diagnosa_id</t>
+  </si>
+  <si>
+    <t>kerusakan_id</t>
+  </si>
+  <si>
+    <t>solusi_id</t>
+  </si>
+  <si>
+    <t>fk aturan gejala</t>
+  </si>
+  <si>
+    <t>fk aturan diagnosa</t>
+  </si>
+  <si>
+    <t>fk aturan solusi</t>
+  </si>
+  <si>
+    <t>fk atura kerusakan</t>
+  </si>
+  <si>
+    <t>id_diagnosa</t>
+  </si>
+  <si>
+    <t>nama_diagnosa</t>
+  </si>
+  <si>
+    <t>id_kerusakan</t>
+  </si>
+  <si>
+    <t>nama_kerusakan</t>
+  </si>
+  <si>
+    <t>id_solusi</t>
+  </si>
+  <si>
+    <t>nama_solusi</t>
   </si>
 </sst>
 </file>
@@ -299,14 +477,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -326,14 +501,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,14 +816,14 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
@@ -653,7 +831,7 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -673,10 +851,10 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
@@ -687,13 +865,13 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
@@ -704,12 +882,12 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
@@ -717,12 +895,12 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="6"/>
@@ -730,12 +908,12 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="6"/>
@@ -743,12 +921,12 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="6"/>
@@ -756,14 +934,14 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="6"/>
@@ -771,12 +949,12 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="6"/>
@@ -784,12 +962,12 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
@@ -797,12 +975,12 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
@@ -821,17 +999,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
@@ -846,28 +1024,28 @@
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
@@ -879,7 +1057,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
@@ -891,7 +1069,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
@@ -903,17 +1081,17 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -927,7 +1105,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
@@ -939,7 +1117,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
@@ -951,7 +1129,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
@@ -964,6 +1142,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A18:A22"/>
@@ -980,11 +1163,6 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -995,7 +1173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1011,23 +1189,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
@@ -1045,195 +1223,195 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="19"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="19"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="19"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1244,4 +1422,679 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>255</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4">
+        <v>255</v>
+      </c>
+      <c r="K4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>255</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7">
+        <v>255</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>255</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <v>255</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10">
+        <v>255</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>255</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11">
+        <v>255</v>
+      </c>
+      <c r="K11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12">
+        <v>255</v>
+      </c>
+      <c r="K12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
+      </c>
+      <c r="K16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17">
+        <v>255</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17">
+        <v>11</v>
+      </c>
+      <c r="K17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20">
+        <v>11</v>
+      </c>
+      <c r="K20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23">
+        <v>255</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24">
+        <v>11</v>
+      </c>
+      <c r="K24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>104</v>
+      </c>
+      <c r="I25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25">
+        <v>255</v>
+      </c>
+      <c r="K25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28">
+        <v>255</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>